<commit_message>
Fixed publish.ini for clinicalreasoning
</commit_message>
<xml_diff>
--- a/old_image/evidencevariable.xlsx
+++ b/old_image/evidencevariable.xlsx
@@ -943,13 +943,13 @@
     <t>Device used for determining characteristic.</t>
   </si>
   <si>
-    <t>EvidenceVariable.characteristic.usageContext</t>
+    <t>EvidenceVariable.characteristic.booleanSet</t>
   </si>
   <si>
     <t>What code/value pairs define members?</t>
   </si>
   <si>
-    <t>Use UsageContext to define the members of the population, such as Age Ranges, Genders, Settings.</t>
+    <t>Use booleanSet to define the members of the population, such as Age Ranges, Genders, Settings.</t>
   </si>
   <si>
     <t>Need to be able to define members more structurally when more information can be communicated such as age range.</t>
@@ -6213,7 +6213,7 @@
         <v>40</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>185</v>
+        <v>120</v>
       </c>
       <c r="K46" t="s" s="2">
         <v>299</v>

</xml_diff>